<commit_message>
class and interface updates
</commit_message>
<xml_diff>
--- a/Assets/Imports/Waves.wavedata.xlsx
+++ b/Assets/Imports/Waves.wavedata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>#author</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>[Saucers]</t>
+  </si>
+  <si>
+    <t>[Time]</t>
   </si>
 </sst>
 </file>
@@ -390,7 +393,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -411,12 +416,18 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add countdown and wave titles
</commit_message>
<xml_diff>
--- a/Assets/Imports/Waves.wavedata.xlsx
+++ b/Assets/Imports/Waves.wavedata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>#author</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>[Time]</t>
+  </si>
+  <si>
+    <t>$startTime</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -415,6 +418,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>30</v>
+      </c>
+    </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
@@ -425,10 +436,98 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>